<commit_message>
#Done 2.1 search for order data
</commit_message>
<xml_diff>
--- a/API/Resources/Template/Report/4.4Report_QRCODE_WIP/Report_QRCODE_WIP.xlsx
+++ b/API/Resources/Template/Report/4.4Report_QRCODE_WIP/Report_QRCODE_WIP.xlsx
@@ -692,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -732,19 +732,40 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -760,6 +781,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -771,39 +795,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1090,7 +1091,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1121,19 +1122,19 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="7"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1">
       <c r="A2" s="7"/>
@@ -1144,87 +1145,87 @@
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
-      <c r="I2" s="30" t="s">
+      <c r="I2" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1">
       <c r="A3" s="7"/>
       <c r="B3" s="12"/>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="17" t="s">
+      <c r="D3" s="28"/>
+      <c r="E3" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23" t="s">
+      <c r="F3" s="29"/>
+      <c r="G3" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="20" t="s">
+      <c r="I3" s="28"/>
+      <c r="J3" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="26" t="s">
+      <c r="K3" s="33"/>
+      <c r="L3" s="34" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="27" customHeight="1">
       <c r="A4" s="7"/>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>81</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="16" t="s">
+      <c r="G4" s="31"/>
+      <c r="H4" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="L4" s="27"/>
+      <c r="L4" s="35"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1">
       <c r="A5" s="7"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="36"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="39" t="s">
         <v>60</v>
       </c>
       <c r="C6" s="13" t="s">
@@ -1281,12 +1282,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:J5"/>
     <mergeCell ref="B1:L1"/>
     <mergeCell ref="I2:L2"/>
     <mergeCell ref="C3:D3"/>
@@ -1298,6 +1293,12 @@
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>